<commit_message>
aggiunti autonomia, prezzo, airbag
</commit_message>
<xml_diff>
--- a/db_auto_usate.xlsx
+++ b/db_auto_usate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Francesco\Santi Francesco\Corsi\Boolean\Esercitazioni pomeridiane\db-first\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CEEA3E-9EA6-4878-B6BD-4FB7B71E20DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C77FCA3-1BA5-408D-93CD-6E8D169DF79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA8C4353-287B-4314-B167-C6CC5B75BB2E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>auto_usate</t>
   </si>
@@ -138,12 +138,6 @@
     <t>tinyint</t>
   </si>
   <si>
-    <t>litri/100km</t>
-  </si>
-  <si>
-    <t>decimal(3, 1)</t>
-  </si>
-  <si>
     <t>notnull, auto_increment, unique</t>
   </si>
   <si>
@@ -154,6 +148,33 @@
   </si>
   <si>
     <t>es. benzina</t>
+  </si>
+  <si>
+    <t>autonomia</t>
+  </si>
+  <si>
+    <t>litri/100km (se alimentazione a combustibile)</t>
+  </si>
+  <si>
+    <t>km (se alimentazione elettrica)</t>
+  </si>
+  <si>
+    <t>airbag</t>
+  </si>
+  <si>
+    <t>carrozzeria</t>
+  </si>
+  <si>
+    <t>varchar(40)</t>
+  </si>
+  <si>
+    <t>es. berlina, SUV ecc.</t>
+  </si>
+  <si>
+    <t>prezzo</t>
+  </si>
+  <si>
+    <t>decimal(4, 1)</t>
   </si>
 </sst>
 </file>
@@ -512,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F793923C-DC58-46DA-82ED-58A551DEF796}">
-  <dimension ref="B4:E24"/>
+  <dimension ref="B4:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +545,7 @@
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -559,7 +580,7 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -570,7 +591,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -581,176 +602,220 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
         <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>14</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>33</v>
       </c>
-      <c r="D24" t="s">
-        <v>37</v>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>